<commit_message>
#4362 ITA_core, #4364 ITA_driver の修正
</commit_message>
<xml_diff>
--- a/oase-root/libs/commonlibs/template.xlsx
+++ b/oase-root/libs/commonlibs/template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\000001A00A6P3\Desktop\mail\EPOCH\sprint5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICF_AutoCapsule_disabled\02.業務\20200930\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21855" windowHeight="9480" tabRatio="601"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21852" windowHeight="9480" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>RuleSet</t>
   </si>
@@ -816,10 +816,6 @@
     <phoneticPr fontId="14"/>
   </si>
   <si>
-    <t>ITA_NAME=action43,SYMPHONY_CLASS_ID=2,OPERATION_ID={{ VAR_test1 }}</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
     <t>2020-01-01 00:00</t>
     <phoneticPr fontId="14"/>
   </si>
@@ -916,14 +912,6 @@
   </si>
   <si>
     <t>ITA(ver1)</t>
-  </si>
-  <si>
-    <t>rule2</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
-    <t>ITA_NAME=action43,SYMPHONY_CLASS_ID=2</t>
-    <phoneticPr fontId="14"/>
   </si>
   <si>
     <t>ITA_NAME=action43,SYMPHONY_CLASS_ID=2,MENU_ID=1,CONVERT_FLG=TRUE</t>
@@ -1248,10 +1236,6 @@
   </si>
   <si>
     <t>rule9</t>
-  </si>
-  <si>
-    <t>ITA_NAME=action43,CONDUCTOR_CLASS_ID=2</t>
-    <phoneticPr fontId="14"/>
   </si>
   <si>
     <t xml:space="preserve">【ITAドライバー】
@@ -1395,6 +1379,51 @@
     <rPh sb="617" eb="619">
       <t>セッテイ</t>
     </rPh>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>^.*エラーが発生しました。.*$</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>rule10</t>
+  </si>
+  <si>
+    <t>ITA_NAME=action43,SYMPHONY_CLASS_ID=2,OPERATION_ID=1</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>ITA_NAME=action43,CONDUCTOR_CLASS_ID=2,OPERATION_ID={{ VAR_test }}</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>ITA_NAME=action43,CONDUCTOR_CLASS_ID=2,OPERATION_ID=2</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>ITA_NAME=action43,CONDUCTOR_CLASS_ID=2,MENU_ID=1,CONVERT_FLG=TRUE</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>ITA_NAME=action43,CONDUCTOR_CLASS_ID=2,MENU_ID=1:2,CONVERT_FLG=FALSE</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>ITA_NAME=action43,SYMPHONY_CLASS_ID=2,OPERATION_ID={{ VAR_test }}</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>rule2</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>rule11</t>
+  </si>
+  <si>
+    <t>rule12</t>
+  </si>
+  <si>
+    <t>^.*エラーが発生しました。.*$</t>
     <phoneticPr fontId="14"/>
   </si>
 </sst>
@@ -2416,16 +2445,16 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="9.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="38" customWidth="1"/>
-    <col min="3" max="17" width="9.140625" style="38" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="38" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="38"/>
+    <col min="1" max="1" width="3.5546875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="38" customWidth="1"/>
+    <col min="3" max="17" width="9.109375" style="38" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="38" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
@@ -2489,7 +2518,7 @@
     <row r="6" spans="2:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="2:13" s="42" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" s="42" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="43"/>
       <c r="C7" s="44"/>
       <c r="D7" s="45"/>
@@ -2503,7 +2532,7 @@
       <c r="L7" s="46"/>
       <c r="M7" s="46"/>
     </row>
-    <row r="8" spans="2:13" s="10" customFormat="1" ht="19.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" s="10" customFormat="1" ht="19.2" x14ac:dyDescent="0.2">
       <c r="B8" s="47"/>
       <c r="C8" s="48" t="s">
         <v>11</v>
@@ -2553,7 +2582,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="2:13" s="10" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" s="10" customFormat="1" ht="38.4" x14ac:dyDescent="0.2">
       <c r="B10" s="53"/>
       <c r="C10" s="54"/>
       <c r="D10" s="7" t="s">
@@ -2717,7 +2746,7 @@
       <c r="L18" s="58"/>
       <c r="M18" s="58"/>
     </row>
-    <row r="19" spans="2:13" ht="10.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="61" t="s">
         <v>25</v>
       </c>
@@ -2751,32 +2780,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="103.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="103.5703125" customWidth="1"/>
-    <col min="8" max="11" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="103.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="103.5546875" customWidth="1"/>
+    <col min="8" max="11" width="2.88671875" customWidth="1"/>
     <col min="12" max="12" width="12" style="6"/>
     <col min="13" max="13" width="12" style="6" customWidth="1"/>
     <col min="14" max="16384" width="12" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="63" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>43</v>
@@ -2791,16 +2820,16 @@
         <v>39</v>
       </c>
       <c r="H2" s="69" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I2" s="69" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J2" s="70" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K2" s="71" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L2" s="64" t="s">
         <v>51</v>
@@ -2809,7 +2838,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>30</v>
       </c>
@@ -2826,7 +2855,7 @@
         <v>49</v>
       </c>
       <c r="F3" s="66" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="G3" s="66" t="s">
         <v>33</v>
@@ -2845,10 +2874,10 @@
       </c>
       <c r="L3" s="12"/>
       <c r="M3" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>30</v>
       </c>
@@ -2856,16 +2885,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F4" s="66" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="G4" s="66" t="s">
         <v>40</v>
@@ -2882,12 +2911,10 @@
       <c r="K4" s="65">
         <v>0</v>
       </c>
-      <c r="L4" s="12" t="s">
-        <v>62</v>
-      </c>
+      <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>30</v>
       </c>
@@ -2898,13 +2925,13 @@
         <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="66" t="s">
         <v>67</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>71</v>
       </c>
       <c r="G5" s="66" t="s">
         <v>40</v>
@@ -2921,10 +2948,12 @@
       <c r="K5" s="65">
         <v>0</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>30</v>
       </c>
@@ -2932,16 +2961,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="F6" s="66" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G6" s="66" t="s">
         <v>40</v>
@@ -2961,7 +2990,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
         <v>30</v>
       </c>
@@ -2969,16 +2998,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="66" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="G7" s="66" t="s">
         <v>40</v>
@@ -2998,7 +3027,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>30</v>
       </c>
@@ -3009,13 +3038,13 @@
         <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="66" t="s">
         <v>69</v>
-      </c>
-      <c r="F8" s="66" t="s">
-        <v>75</v>
       </c>
       <c r="G8" s="66" t="s">
         <v>40</v>
@@ -3035,7 +3064,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>30</v>
       </c>
@@ -3046,13 +3075,13 @@
         <v>31</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G9" s="66" t="s">
         <v>40</v>
@@ -3072,7 +3101,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>30</v>
       </c>
@@ -3080,19 +3109,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="G10" s="66" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="H10" s="65">
         <v>1</v>
@@ -3101,17 +3130,15 @@
         <v>1</v>
       </c>
       <c r="J10" s="65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="65">
-        <v>1</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>62</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>30</v>
       </c>
@@ -3119,16 +3146,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="G11" s="66" t="s">
         <v>40</v>
@@ -3140,141 +3167,254 @@
         <v>1</v>
       </c>
       <c r="J11" s="65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" s="65">
-        <v>2</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="67">
+        <v>10</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="65">
+        <v>1</v>
+      </c>
+      <c r="I12" s="65">
+        <v>1</v>
+      </c>
+      <c r="J12" s="65">
+        <v>0</v>
+      </c>
+      <c r="K12" s="65">
+        <v>0</v>
+      </c>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="12"/>
+    <row r="13" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="67">
+        <v>11</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="65">
+        <v>1</v>
+      </c>
+      <c r="I13" s="65">
+        <v>1</v>
+      </c>
+      <c r="J13" s="65">
+        <v>1</v>
+      </c>
+      <c r="K13" s="65">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" ht="97.5" x14ac:dyDescent="0.2">
-      <c r="B15" s="33" t="s">
+    <row r="14" spans="1:13" s="18" customFormat="1" ht="12.6" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="67">
+        <v>12</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="65">
+        <v>1</v>
+      </c>
+      <c r="I14" s="65">
+        <v>1</v>
+      </c>
+      <c r="J14" s="65">
+        <v>2</v>
+      </c>
+      <c r="K14" s="65">
+        <v>2</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="2:13" ht="90" x14ac:dyDescent="0.2">
+      <c r="B18" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C18" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D18" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E18" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F18" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="H15" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="M15" s="35" t="s">
+      <c r="G18" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="C16" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="34"/>
-    </row>
-    <row r="17" spans="6:7" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="F17" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="34"/>
-    </row>
-    <row r="18" spans="6:7" ht="97.5" x14ac:dyDescent="0.2">
-      <c r="F18" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="M18" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="144" x14ac:dyDescent="0.25">
+      <c r="C19" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>87</v>
+      </c>
       <c r="G19" s="34"/>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-    </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" ht="153" x14ac:dyDescent="0.25">
+      <c r="F20" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="F21" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
     </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H18:K18"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E12:E13">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E15:E16">
       <formula1>"ITA,mail"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E3:E11">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E3:E14">
       <formula1>"ITA(ver1),mail(ver1)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3291,14 +3431,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3309,7 +3449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3320,7 +3460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3332,7 +3472,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>